<commit_message>
Common header and footer
</commit_message>
<xml_diff>
--- a/Members_Detail/Members Detail.xlsx
+++ b/Members_Detail/Members Detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prana\Desktop\Robocon\Website\Official-Website-2022\Members_Detail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EE5DBA-DFDC-466F-96A6-84CBB8178B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343191E2-80B3-496C-B712-105B345F5F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{63D6346B-1086-495A-8E73-398F698D2E3C}"/>
   </bookViews>
@@ -392,15 +392,6 @@
     <t>Rehana</t>
   </si>
   <si>
-    <t>Ex-SIESED Lead</t>
-  </si>
-  <si>
-    <t>Ex-Team Lead</t>
-  </si>
-  <si>
-    <t>Ex-SPACED Lead</t>
-  </si>
-  <si>
     <t>Adheesh Mathur</t>
   </si>
   <si>
@@ -410,9 +401,6 @@
     <t>https://instagram.com/_adheesh.1210_?igshid=ZDdkNTZiNTM=/</t>
   </si>
   <si>
-    <t>Ex-SAMBED Lead</t>
-  </si>
-  <si>
     <t>Pranav Malakar</t>
   </si>
   <si>
@@ -495,6 +483,18 @@
   </si>
   <si>
     <t>https://instagram.com/daaaaanu?igshid=MjEwN2IyYWYwYw==/</t>
+  </si>
+  <si>
+    <t>Team Lead 2023</t>
+  </si>
+  <si>
+    <t>SAMBED Lead 2023</t>
+  </si>
+  <si>
+    <t>SPACED Lead 2023</t>
+  </si>
+  <si>
+    <t>SIESED Lead 2023</t>
   </si>
 </sst>
 </file>
@@ -1137,17 +1137,17 @@
     </row>
     <row r="8" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1290,17 +1290,17 @@
     </row>
     <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="53.4" x14ac:dyDescent="0.3">
@@ -1335,7 +1335,7 @@
     </row>
     <row r="8" spans="1:5" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>112</v>
@@ -1473,17 +1473,17 @@
     </row>
     <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1733,7 +1733,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1766,7 +1766,7 @@
         <v>113</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6" t="s">
@@ -1778,17 +1778,17 @@
     </row>
     <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="27" x14ac:dyDescent="0.3">
@@ -1796,7 +1796,7 @@
         <v>116</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1804,90 +1804,90 @@
     </row>
     <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>